<commit_message>
Update PMP Replay Zoom Links 2024.xlsx
</commit_message>
<xml_diff>
--- a/PMP Replay Zoom Links 2024.xlsx
+++ b/PMP Replay Zoom Links 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://skillsoft-my.sharepoint.com/personal/carl_mullin_skillsoft_com/Documents/Desktop as of Aug 2023/PMP ATP Bootcamp Documents for Percipio/Replays/Not Password Protected/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://americanredcross-my.sharepoint.com/personal/trenton_anderson_redcross_org/Documents/Documents/GitHub/PMPReplay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:8001_{ADFF34E3-F321-4B5E-9B4A-FF7203E6D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{317CF296-9908-416C-930F-D0922907B0D4}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:8001_{ADFF34E3-F321-4B5E-9B4A-FF7203E6D563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{805C6F2A-0E29-4C7E-88DC-C2F3A9F4E573}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9270DAD-5426-4C94-A2EA-23A7872E7F65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9270DAD-5426-4C94-A2EA-23A7872E7F65}"/>
   </bookViews>
   <sheets>
     <sheet name="NovDecJan 2024 ICE" sheetId="44" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="417">
   <si>
     <t>PMP Bootcamp NA 8-Day Cohort</t>
   </si>
@@ -1311,6 +1311,9 @@
   </si>
   <si>
     <t>https://skillsoftbootcamp.zoom.us/rec/share/LxNN6pb5ZS7MmgmHkerpYdpxJa6Jtwa9tmcRvnQTDAWIIRqYj3sATvbLfYG5NXBV.HfhAmZrW1QY40ETI</t>
+  </si>
+  <si>
+    <t>pmpBootcampReplay!</t>
   </si>
 </sst>
 </file>
@@ -1739,10 +1742,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1884,8 +1887,14 @@
         <v>303</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>416</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5904,6 +5913,64 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Links xmlns="b0bb338f-7b42-4437-b836-3bba46acea74">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Links>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b0bb338f-7b42-4437-b836-3bba46acea74">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="567d2312-0729-48ba-857e-77359d3146cd" xsi:nil="true"/>
+    <SharedWithUsers xmlns="847b69b4-afc2-4d71-b6dd-a5b5c23f9e3f">
+      <UserInfo>
+        <DisplayName>Greg Fuller</DisplayName>
+        <AccountId>182</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Carl Mullin</DisplayName>
+        <AccountId>194</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Chris Keenan</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Eian Clair</DisplayName>
+        <AccountId>1894</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dave Robichaud</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mohammed Irfan Ahmed</DisplayName>
+        <AccountId>1864</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C72DEC5C8BF5284E81BD4C5AED9FC143" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c5b3b49520133842085f6f075fab84">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="b0bb338f-7b42-4437-b836-3bba46acea74" xmlns:ns3="847b69b4-afc2-4d71-b6dd-a5b5c23f9e3f" xmlns:ns4="567d2312-0729-48ba-857e-77359d3146cd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a1cdef1588082fadd852b6af67ae834" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6187,81 +6254,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Links xmlns="b0bb338f-7b42-4437-b836-3bba46acea74">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Links>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b0bb338f-7b42-4437-b836-3bba46acea74">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="567d2312-0729-48ba-857e-77359d3146cd" xsi:nil="true"/>
-    <SharedWithUsers xmlns="847b69b4-afc2-4d71-b6dd-a5b5c23f9e3f">
-      <UserInfo>
-        <DisplayName>Greg Fuller</DisplayName>
-        <AccountId>182</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Carl Mullin</DisplayName>
-        <AccountId>194</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Chris Keenan</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Eian Clair</DisplayName>
-        <AccountId>1894</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dave Robichaud</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mohammed Irfan Ahmed</DisplayName>
-        <AccountId>1864</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7404C892-7738-408C-B9B8-B63D959B9347}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FB28207-7E0F-4498-8448-D078A1B0B685}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="b0bb338f-7b42-4437-b836-3bba46acea74"/>
-    <ds:schemaRef ds:uri="847b69b4-afc2-4d71-b6dd-a5b5c23f9e3f"/>
-    <ds:schemaRef ds:uri="567d2312-0729-48ba-857e-77359d3146cd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6286,9 +6282,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FB28207-7E0F-4498-8448-D078A1B0B685}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7404C892-7738-408C-B9B8-B63D959B9347}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="b0bb338f-7b42-4437-b836-3bba46acea74"/>
+    <ds:schemaRef ds:uri="847b69b4-afc2-4d71-b6dd-a5b5c23f9e3f"/>
+    <ds:schemaRef ds:uri="567d2312-0729-48ba-857e-77359d3146cd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>